<commit_message>
changes related to validation
</commit_message>
<xml_diff>
--- a/src/assets/extra/AIR_CONSOLE_FORMAT.xlsx
+++ b/src/assets/extra/AIR_CONSOLE_FORMAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myWorkStarted\tarifftales-spa-app\src\assets\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2D6A30-6317-4F4D-8BC6-FAB3FDD9799D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B9759C-B3AC-491E-9AB7-1E653AB8A520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>Commodity</t>
   </si>
@@ -104,12 +104,6 @@
     <t>NRate</t>
   </si>
   <si>
-    <t>ALL Flights</t>
-  </si>
-  <si>
-    <t>EXCEPT 6E 0213,2443</t>
-  </si>
-  <si>
     <t>CONTRACT</t>
   </si>
   <si>
@@ -141,6 +135,33 @@
   </si>
   <si>
     <t>final check</t>
+  </si>
+  <si>
+    <t>Uk 347</t>
+  </si>
+  <si>
+    <t>Before 07:40</t>
+  </si>
+  <si>
+    <t>Uk 345</t>
+  </si>
+  <si>
+    <t>For All Flights departed between 09:01 TO 23:59 HRS</t>
+  </si>
+  <si>
+    <t>For All Flights between 15:00 HRS TILL 23:59 HRS</t>
+  </si>
+  <si>
+    <t>07:30</t>
+  </si>
+  <si>
+    <t>09:01 TO 23:59 HRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15:00 HRS - 23:59 HRS</t>
+  </si>
+  <si>
+    <t>MON,TUE,WED,THU,FRI,SAT,SUN</t>
   </si>
 </sst>
 </file>
@@ -151,7 +172,7 @@
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -225,6 +246,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -273,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -320,6 +356,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +580,7 @@
   <dimension ref="A1:S999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -623,10 +665,10 @@
     </row>
     <row r="2" spans="1:19" ht="15.6">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="16">
         <v>44380</v>
@@ -635,36 +677,38 @@
         <v>44382</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J2" s="3">
         <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>34</v>
+      </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1" t="s">
         <v>15</v>
@@ -678,10 +722,10 @@
     </row>
     <row r="3" spans="1:19" ht="15.6">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="16">
         <v>44380</v>
@@ -690,36 +734,38 @@
         <v>44383</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J3" s="3">
         <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>36</v>
+      </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="1" t="s">
         <v>15</v>
@@ -733,10 +779,10 @@
     </row>
     <row r="4" spans="1:19" ht="15.6">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="16">
         <v>44380</v>
@@ -745,34 +791,37 @@
         <v>44384</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J4" s="3">
         <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" s="14" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>37</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="1" t="s">
@@ -787,10 +836,10 @@
     </row>
     <row r="5" spans="1:19" ht="15.6">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="16">
         <v>44380</v>
@@ -799,34 +848,37 @@
         <v>44385</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J5" s="3">
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>23</v>
+        <v>28</v>
+      </c>
+      <c r="N5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>38</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="1" t="s">
@@ -841,10 +893,10 @@
     </row>
     <row r="6" spans="1:19" ht="15.6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="16">
         <v>44380</v>
@@ -853,36 +905,38 @@
         <v>44386</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J6" s="3">
         <v>2</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>39</v>
+      </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="1" t="s">
         <v>15</v>
@@ -896,10 +950,10 @@
     </row>
     <row r="7" spans="1:19" ht="15.6">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="16">
         <v>44380</v>
@@ -908,36 +962,38 @@
         <v>44387</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J7" s="3">
         <v>2</v>
       </c>
       <c r="K7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>30</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="1" t="s">
         <v>15</v>
@@ -951,10 +1007,10 @@
     </row>
     <row r="8" spans="1:19" ht="15.6">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="16">
         <v>44380</v>
@@ -963,36 +1019,38 @@
         <v>44388</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="3">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="I8" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="J8" s="3">
         <v>2</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M8" t="s">
-        <v>30</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="N8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>40</v>
+      </c>
       <c r="Q8" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
air line charges implemented..
</commit_message>
<xml_diff>
--- a/src/assets/extra/AIR_CONSOLE_FORMAT.xlsx
+++ b/src/assets/extra/AIR_CONSOLE_FORMAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myWorkStarted\tarifftales-spa-app\src\assets\extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UP_WORK_PROJECTS\TariffTales_project\tarifftales-spa-app\src\assets\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B9759C-B3AC-491E-9AB7-1E653AB8A520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAC0606-916A-4277-A236-A4CCBB58F321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSOLE" sheetId="1" r:id="rId1"/>
@@ -309,7 +309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -362,6 +362,15 @@
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -599,8 +608,8 @@
     <col min="12" max="12" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="16.3984375" customWidth="1"/>
     <col min="14" max="14" width="26.19921875" customWidth="1"/>
-    <col min="15" max="15" width="29.5" customWidth="1"/>
-    <col min="16" max="16" width="19" customWidth="1"/>
+    <col min="15" max="15" width="29.5" style="24" customWidth="1"/>
+    <col min="16" max="16" width="19" style="24" customWidth="1"/>
     <col min="17" max="27" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -647,10 +656,10 @@
       <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="22" t="s">
         <v>10</v>
       </c>
       <c r="Q1" s="8" t="s">
@@ -709,7 +718,7 @@
       <c r="O2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="25"/>
       <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
@@ -766,7 +775,7 @@
       <c r="O3" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="3"/>
+      <c r="P3" s="26"/>
       <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
@@ -823,7 +832,7 @@
       <c r="O4" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="26"/>
       <c r="Q4" s="1" t="s">
         <v>15</v>
       </c>
@@ -880,7 +889,7 @@
       <c r="O5" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="26"/>
       <c r="Q5" s="1" t="s">
         <v>15</v>
       </c>
@@ -937,7 +946,7 @@
       <c r="O6" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="26"/>
       <c r="Q6" s="1" t="s">
         <v>15</v>
       </c>
@@ -994,7 +1003,7 @@
       <c r="O7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="26"/>
       <c r="Q7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1071,7 +1080,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="1"/>
       <c r="N9" s="1"/>
-      <c r="O9" s="14"/>
+      <c r="O9" s="23"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
@@ -1086,7 +1095,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="14"/>
+      <c r="O10" s="23"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
@@ -1102,7 +1111,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="O11" s="14"/>
+      <c r="O11" s="23"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="15"/>
       <c r="S11" s="15"/>
@@ -1117,7 +1126,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="1"/>
       <c r="N12" s="1"/>
-      <c r="O12" s="14"/>
+      <c r="O12" s="23"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
@@ -1132,7 +1141,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="O13" s="14"/>
+      <c r="O13" s="23"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="15"/>
       <c r="S13" s="15"/>
@@ -1147,7 +1156,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="O14" s="14"/>
+      <c r="O14" s="23"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="15"/>
       <c r="S14" s="15"/>
@@ -1162,7 +1171,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="O15" s="14"/>
+      <c r="O15" s="23"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
@@ -1177,7 +1186,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="O16" s="14"/>
+      <c r="O16" s="23"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="15"/>
       <c r="S16" s="15"/>
@@ -1192,7 +1201,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="14"/>
+      <c r="O17" s="23"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="15"/>
       <c r="S17" s="15"/>
@@ -1208,7 +1217,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="O18" s="14"/>
+      <c r="O18" s="23"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
@@ -1224,7 +1233,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="1"/>
       <c r="N19" s="1"/>
-      <c r="O19" s="14"/>
+      <c r="O19" s="23"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="15"/>
       <c r="S19" s="15"/>
@@ -1241,7 +1250,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="14"/>
+      <c r="O20" s="23"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="15"/>
       <c r="S20" s="15"/>
@@ -1258,7 +1267,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="14"/>
+      <c r="O21" s="23"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
@@ -1275,7 +1284,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="14"/>
+      <c r="O22" s="23"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
@@ -1292,7 +1301,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="1"/>
       <c r="N23" s="1"/>
-      <c r="O23" s="14"/>
+      <c r="O23" s="23"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
@@ -1309,7 +1318,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="1"/>
       <c r="N24" s="1"/>
-      <c r="O24" s="14"/>
+      <c r="O24" s="23"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
@@ -1326,7 +1335,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="1"/>
       <c r="N25" s="1"/>
-      <c r="O25" s="14"/>
+      <c r="O25" s="23"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
@@ -1343,7 +1352,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="1"/>
       <c r="N26" s="1"/>
-      <c r="O26" s="14"/>
+      <c r="O26" s="23"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
@@ -1360,7 +1369,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="1"/>
       <c r="N27" s="1"/>
-      <c r="O27" s="14"/>
+      <c r="O27" s="23"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
@@ -1377,7 +1386,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="1"/>
       <c r="N28" s="1"/>
-      <c r="O28" s="14"/>
+      <c r="O28" s="23"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
@@ -1394,7 +1403,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="1"/>
       <c r="N29" s="1"/>
-      <c r="O29" s="14"/>
+      <c r="O29" s="23"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
@@ -1411,7 +1420,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="1"/>
       <c r="N30" s="1"/>
-      <c r="O30" s="14"/>
+      <c r="O30" s="23"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
@@ -1428,7 +1437,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="1"/>
       <c r="N31" s="1"/>
-      <c r="O31" s="14"/>
+      <c r="O31" s="23"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
@@ -1445,7 +1454,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="1"/>
       <c r="N32" s="1"/>
-      <c r="O32" s="14"/>
+      <c r="O32" s="23"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
@@ -1462,7 +1471,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="14"/>
+      <c r="O33" s="23"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
@@ -1479,7 +1488,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="1"/>
       <c r="N34" s="1"/>
-      <c r="O34" s="14"/>
+      <c r="O34" s="23"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
@@ -1496,7 +1505,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="1"/>
       <c r="N35" s="1"/>
-      <c r="O35" s="14"/>
+      <c r="O35" s="23"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="15"/>
       <c r="S35" s="15"/>
@@ -1513,7 +1522,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="1"/>
       <c r="N36" s="1"/>
-      <c r="O36" s="14"/>
+      <c r="O36" s="23"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="15"/>
       <c r="S36" s="15"/>
@@ -1530,7 +1539,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="1"/>
       <c r="N37" s="1"/>
-      <c r="O37" s="14"/>
+      <c r="O37" s="23"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
@@ -1547,7 +1556,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="1"/>
       <c r="N38" s="1"/>
-      <c r="O38" s="14"/>
+      <c r="O38" s="23"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
@@ -1564,7 +1573,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="1"/>
       <c r="N39" s="1"/>
-      <c r="O39" s="14"/>
+      <c r="O39" s="23"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
@@ -1581,7 +1590,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="1"/>
       <c r="N40" s="1"/>
-      <c r="O40" s="14"/>
+      <c r="O40" s="23"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="15"/>
       <c r="S40" s="15"/>
@@ -1598,7 +1607,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="1"/>
       <c r="N41" s="1"/>
-      <c r="O41" s="14"/>
+      <c r="O41" s="23"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="15"/>
       <c r="S41" s="15"/>
@@ -1615,7 +1624,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="O42" s="14"/>
+      <c r="O42" s="23"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="15"/>
       <c r="S42" s="15"/>
@@ -1632,7 +1641,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="14"/>
+      <c r="O43" s="23"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="15"/>
       <c r="S43" s="15"/>
@@ -1649,7 +1658,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="1"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="14"/>
+      <c r="O44" s="23"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="15"/>
       <c r="S44" s="15"/>
@@ -1666,7 +1675,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="14"/>
+      <c r="O45" s="23"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="15"/>
       <c r="S45" s="15"/>
@@ -1683,7 +1692,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="14"/>
+      <c r="O46" s="23"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -1700,7 +1709,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="14"/>
+      <c r="O47" s="23"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="15"/>
       <c r="S47" s="15"/>
@@ -1717,7 +1726,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="14"/>
+      <c r="O48" s="23"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="15"/>
       <c r="S48" s="15"/>
@@ -1782,7 +1791,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="14"/>
+      <c r="O52" s="23"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="15"/>
       <c r="S52" s="15"/>
@@ -1799,7 +1808,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="1"/>
       <c r="N53" s="1"/>
-      <c r="O53" s="14"/>
+      <c r="O53" s="23"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="15"/>
       <c r="S53" s="15"/>
@@ -1816,7 +1825,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54" s="14"/>
+      <c r="O54" s="23"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="15"/>
       <c r="S54" s="15"/>
@@ -1833,7 +1842,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="1"/>
       <c r="N55" s="1"/>
-      <c r="O55" s="14"/>
+      <c r="O55" s="23"/>
       <c r="Q55" s="1"/>
       <c r="R55" s="15"/>
       <c r="S55" s="15"/>
@@ -1850,7 +1859,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="14"/>
+      <c r="O56" s="23"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
@@ -1867,7 +1876,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="14"/>
+      <c r="O57" s="23"/>
       <c r="Q57" s="1"/>
       <c r="R57" s="15"/>
       <c r="S57" s="15"/>
@@ -1884,7 +1893,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="1"/>
       <c r="N58" s="1"/>
-      <c r="O58" s="14"/>
+      <c r="O58" s="23"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="15"/>
       <c r="S58" s="15"/>
@@ -1901,7 +1910,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="1"/>
       <c r="N59" s="1"/>
-      <c r="O59" s="14"/>
+      <c r="O59" s="23"/>
       <c r="Q59" s="1"/>
       <c r="R59" s="15"/>
       <c r="S59" s="15"/>
@@ -1918,7 +1927,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="1"/>
       <c r="N60" s="1"/>
-      <c r="O60" s="14"/>
+      <c r="O60" s="23"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="15"/>
       <c r="S60" s="15"/>
@@ -1935,7 +1944,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="1"/>
       <c r="N61" s="1"/>
-      <c r="O61" s="14"/>
+      <c r="O61" s="23"/>
       <c r="Q61" s="1"/>
       <c r="R61" s="15"/>
       <c r="S61" s="15"/>
@@ -1952,7 +1961,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="1"/>
       <c r="N62" s="1"/>
-      <c r="O62" s="14"/>
+      <c r="O62" s="23"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="15"/>
       <c r="S62" s="15"/>
@@ -1969,7 +1978,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="1"/>
       <c r="N63" s="1"/>
-      <c r="O63" s="14"/>
+      <c r="O63" s="23"/>
       <c r="Q63" s="1"/>
       <c r="R63" s="15"/>
       <c r="S63" s="15"/>
@@ -1986,7 +1995,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="1"/>
       <c r="N64" s="1"/>
-      <c r="O64" s="14"/>
+      <c r="O64" s="23"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="15"/>
       <c r="S64" s="15"/>
@@ -2003,7 +2012,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="1"/>
       <c r="N65" s="1"/>
-      <c r="O65" s="14"/>
+      <c r="O65" s="23"/>
       <c r="Q65" s="1"/>
       <c r="R65" s="15"/>
       <c r="S65" s="15"/>
@@ -2590,7 +2599,7 @@
       <c r="K104" s="5"/>
       <c r="L104" s="1"/>
       <c r="N104" s="5"/>
-      <c r="O104" s="14"/>
+      <c r="O104" s="23"/>
       <c r="Q104" s="1"/>
       <c r="R104" s="15"/>
       <c r="S104" s="15"/>
@@ -2607,7 +2616,7 @@
       <c r="K105" s="5"/>
       <c r="L105" s="1"/>
       <c r="N105" s="5"/>
-      <c r="O105" s="14"/>
+      <c r="O105" s="23"/>
       <c r="Q105" s="1"/>
       <c r="R105" s="15"/>
       <c r="S105" s="15"/>
@@ -2624,7 +2633,7 @@
       <c r="K106" s="5"/>
       <c r="L106" s="1"/>
       <c r="N106" s="5"/>
-      <c r="O106" s="14"/>
+      <c r="O106" s="23"/>
       <c r="Q106" s="1"/>
       <c r="R106" s="15"/>
       <c r="S106" s="15"/>
@@ -2641,7 +2650,7 @@
       <c r="K107" s="5"/>
       <c r="L107" s="1"/>
       <c r="N107" s="5"/>
-      <c r="O107" s="14"/>
+      <c r="O107" s="23"/>
       <c r="Q107" s="1"/>
       <c r="R107" s="15"/>
       <c r="S107" s="15"/>
@@ -2658,7 +2667,7 @@
       <c r="K108" s="5"/>
       <c r="L108" s="1"/>
       <c r="N108" s="5"/>
-      <c r="O108" s="14"/>
+      <c r="O108" s="23"/>
       <c r="Q108" s="1"/>
       <c r="R108" s="15"/>
       <c r="S108" s="15"/>
@@ -2675,7 +2684,7 @@
       <c r="K109" s="5"/>
       <c r="L109" s="1"/>
       <c r="N109" s="5"/>
-      <c r="O109" s="14"/>
+      <c r="O109" s="23"/>
       <c r="Q109" s="1"/>
       <c r="R109" s="15"/>
       <c r="S109" s="15"/>
@@ -2692,7 +2701,7 @@
       <c r="K110" s="5"/>
       <c r="L110" s="1"/>
       <c r="N110" s="5"/>
-      <c r="O110" s="14"/>
+      <c r="O110" s="23"/>
       <c r="Q110" s="1"/>
       <c r="R110" s="15"/>
       <c r="S110" s="15"/>
@@ -2709,7 +2718,7 @@
       <c r="K111" s="5"/>
       <c r="L111" s="1"/>
       <c r="N111" s="5"/>
-      <c r="O111" s="14"/>
+      <c r="O111" s="23"/>
       <c r="Q111" s="1"/>
       <c r="R111" s="15"/>
       <c r="S111" s="15"/>
@@ -2726,7 +2735,7 @@
       <c r="K112" s="5"/>
       <c r="L112" s="1"/>
       <c r="N112" s="5"/>
-      <c r="O112" s="14"/>
+      <c r="O112" s="23"/>
       <c r="Q112" s="1"/>
       <c r="R112" s="15"/>
       <c r="S112" s="15"/>
@@ -2743,7 +2752,7 @@
       <c r="K113" s="5"/>
       <c r="L113" s="1"/>
       <c r="N113" s="5"/>
-      <c r="O113" s="14"/>
+      <c r="O113" s="23"/>
       <c r="Q113" s="1"/>
       <c r="R113" s="15"/>
       <c r="S113" s="15"/>
@@ -2760,7 +2769,7 @@
       <c r="K114" s="5"/>
       <c r="L114" s="1"/>
       <c r="N114" s="5"/>
-      <c r="O114" s="14"/>
+      <c r="O114" s="23"/>
       <c r="Q114" s="1"/>
       <c r="R114" s="15"/>
       <c r="S114" s="15"/>
@@ -2777,7 +2786,7 @@
       <c r="K115" s="5"/>
       <c r="L115" s="1"/>
       <c r="N115" s="5"/>
-      <c r="O115" s="14"/>
+      <c r="O115" s="23"/>
       <c r="Q115" s="1"/>
       <c r="R115" s="15"/>
       <c r="S115" s="15"/>
@@ -2794,7 +2803,7 @@
       <c r="K116" s="5"/>
       <c r="L116" s="1"/>
       <c r="N116" s="5"/>
-      <c r="O116" s="14"/>
+      <c r="O116" s="23"/>
       <c r="Q116" s="1"/>
       <c r="R116" s="15"/>
       <c r="S116" s="15"/>
@@ -2811,7 +2820,7 @@
       <c r="K117" s="5"/>
       <c r="L117" s="1"/>
       <c r="N117" s="5"/>
-      <c r="O117" s="14"/>
+      <c r="O117" s="23"/>
       <c r="Q117" s="1"/>
       <c r="R117" s="15"/>
       <c r="S117" s="15"/>
@@ -2828,7 +2837,7 @@
       <c r="K118" s="5"/>
       <c r="L118" s="1"/>
       <c r="N118" s="5"/>
-      <c r="O118" s="14"/>
+      <c r="O118" s="23"/>
       <c r="Q118" s="1"/>
       <c r="R118" s="15"/>
       <c r="S118" s="15"/>
@@ -2845,7 +2854,7 @@
       <c r="K119" s="5"/>
       <c r="L119" s="1"/>
       <c r="N119" s="5"/>
-      <c r="O119" s="14"/>
+      <c r="O119" s="23"/>
       <c r="Q119" s="1"/>
       <c r="R119" s="15"/>
       <c r="S119" s="15"/>
@@ -2862,7 +2871,7 @@
       <c r="K120" s="5"/>
       <c r="L120" s="1"/>
       <c r="N120" s="5"/>
-      <c r="O120" s="14"/>
+      <c r="O120" s="23"/>
       <c r="Q120" s="1"/>
       <c r="R120" s="15"/>
       <c r="S120" s="15"/>
@@ -2879,7 +2888,7 @@
       <c r="K121" s="5"/>
       <c r="L121" s="1"/>
       <c r="N121" s="5"/>
-      <c r="O121" s="14"/>
+      <c r="O121" s="23"/>
       <c r="Q121" s="1"/>
       <c r="R121" s="15"/>
       <c r="S121" s="15"/>
@@ -2896,7 +2905,7 @@
       <c r="K122" s="5"/>
       <c r="L122" s="1"/>
       <c r="N122" s="5"/>
-      <c r="O122" s="14"/>
+      <c r="O122" s="23"/>
       <c r="Q122" s="1"/>
       <c r="R122" s="15"/>
       <c r="S122" s="15"/>
@@ -2913,7 +2922,7 @@
       <c r="K123" s="5"/>
       <c r="L123" s="1"/>
       <c r="N123" s="5"/>
-      <c r="O123" s="14"/>
+      <c r="O123" s="23"/>
       <c r="Q123" s="1"/>
       <c r="R123" s="15"/>
       <c r="S123" s="15"/>
@@ -2930,7 +2939,7 @@
       <c r="K124" s="5"/>
       <c r="L124" s="1"/>
       <c r="N124" s="5"/>
-      <c r="O124" s="14"/>
+      <c r="O124" s="23"/>
       <c r="Q124" s="1"/>
       <c r="R124" s="15"/>
       <c r="S124" s="15"/>
@@ -2947,7 +2956,7 @@
       <c r="K125" s="5"/>
       <c r="L125" s="1"/>
       <c r="N125" s="5"/>
-      <c r="O125" s="14"/>
+      <c r="O125" s="23"/>
       <c r="Q125" s="1"/>
       <c r="R125" s="15"/>
       <c r="S125" s="15"/>
@@ -2964,7 +2973,7 @@
       <c r="K126" s="5"/>
       <c r="L126" s="1"/>
       <c r="N126" s="5"/>
-      <c r="O126" s="14"/>
+      <c r="O126" s="23"/>
       <c r="Q126" s="1"/>
       <c r="R126" s="15"/>
       <c r="S126" s="15"/>
@@ -2981,7 +2990,7 @@
       <c r="K127" s="5"/>
       <c r="L127" s="1"/>
       <c r="N127" s="5"/>
-      <c r="O127" s="14"/>
+      <c r="O127" s="23"/>
       <c r="Q127" s="1"/>
       <c r="R127" s="15"/>
       <c r="S127" s="15"/>
@@ -2998,7 +3007,7 @@
       <c r="K128" s="5"/>
       <c r="L128" s="1"/>
       <c r="N128" s="5"/>
-      <c r="O128" s="14"/>
+      <c r="O128" s="23"/>
       <c r="Q128" s="1"/>
       <c r="R128" s="15"/>
       <c r="S128" s="15"/>
@@ -3015,7 +3024,7 @@
       <c r="K129" s="5"/>
       <c r="L129" s="1"/>
       <c r="N129" s="5"/>
-      <c r="O129" s="14"/>
+      <c r="O129" s="23"/>
       <c r="Q129" s="1"/>
       <c r="R129" s="15"/>
       <c r="S129" s="15"/>
@@ -3032,7 +3041,7 @@
       <c r="K130" s="5"/>
       <c r="L130" s="1"/>
       <c r="N130" s="5"/>
-      <c r="O130" s="14"/>
+      <c r="O130" s="23"/>
       <c r="Q130" s="1"/>
       <c r="R130" s="15"/>
       <c r="S130" s="15"/>
@@ -3049,7 +3058,7 @@
       <c r="K131" s="5"/>
       <c r="L131" s="1"/>
       <c r="N131" s="5"/>
-      <c r="O131" s="14"/>
+      <c r="O131" s="23"/>
       <c r="Q131" s="1"/>
       <c r="R131" s="15"/>
       <c r="S131" s="15"/>
@@ -3066,7 +3075,7 @@
       <c r="K132" s="5"/>
       <c r="L132" s="1"/>
       <c r="N132" s="5"/>
-      <c r="O132" s="14"/>
+      <c r="O132" s="23"/>
       <c r="Q132" s="1"/>
       <c r="R132" s="15"/>
       <c r="S132" s="15"/>
@@ -3083,7 +3092,7 @@
       <c r="K133" s="5"/>
       <c r="L133" s="1"/>
       <c r="N133" s="5"/>
-      <c r="O133" s="14"/>
+      <c r="O133" s="23"/>
       <c r="Q133" s="1"/>
       <c r="R133" s="15"/>
       <c r="S133" s="15"/>
@@ -3100,7 +3109,7 @@
       <c r="K134" s="5"/>
       <c r="L134" s="1"/>
       <c r="N134" s="5"/>
-      <c r="O134" s="14"/>
+      <c r="O134" s="23"/>
       <c r="Q134" s="1"/>
       <c r="R134" s="15"/>
       <c r="S134" s="15"/>
@@ -3117,7 +3126,7 @@
       <c r="K135" s="5"/>
       <c r="L135" s="1"/>
       <c r="N135" s="5"/>
-      <c r="O135" s="14"/>
+      <c r="O135" s="23"/>
       <c r="Q135" s="1"/>
       <c r="R135" s="15"/>
       <c r="S135" s="15"/>
@@ -3134,7 +3143,7 @@
       <c r="K136" s="5"/>
       <c r="L136" s="1"/>
       <c r="N136" s="5"/>
-      <c r="O136" s="14"/>
+      <c r="O136" s="23"/>
       <c r="Q136" s="1"/>
       <c r="R136" s="15"/>
       <c r="S136" s="15"/>

</xml_diff>